<commit_message>
- added support for editing weapon/armor modifier - added some debug options
</commit_message>
<xml_diff>
--- a/xml scheme.xlsx
+++ b/xml scheme.xlsx
@@ -5,18 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Visual Studio 2017\Projects\D-OS Save Editor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Visual Studio 2017\Projects\D-OS SE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5618D9-4D03-4C66-8D59-FF6465BCA18B}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6799634D-6A39-4392-A32B-9D557B248801}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23190" windowHeight="10815" xr2:uid="{74786857-5191-4C0D-86D0-001FA1C9B969}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23190" windowHeight="10815" activeTab="4" xr2:uid="{74786857-5191-4C0D-86D0-001FA1C9B969}"/>
   </bookViews>
   <sheets>
     <sheet name="Abilities" sheetId="1" r:id="rId1"/>
     <sheet name="Attributes" sheetId="4" r:id="rId2"/>
     <sheet name="Traits" sheetId="2" r:id="rId3"/>
     <sheet name="Talent" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="242">
   <si>
     <t>bow</t>
   </si>
@@ -388,13 +390,379 @@
   </si>
   <si>
     <t xml:space="preserve">            SingleHanded</t>
+  </si>
+  <si>
+    <t>Armor_Boost_STR_Mod_Ring</t>
+  </si>
+  <si>
+    <t>Armor__</t>
+  </si>
+  <si>
+    <t>Armor__Ring_Boost_Telekinesis_Mod</t>
+  </si>
+  <si>
+    <t>Weapon_Small_WaterDamage_ModSword</t>
+  </si>
+  <si>
+    <t>Weapon_Small_Crit_Mod</t>
+  </si>
+  <si>
+    <t>Armor__Amulet_Boost_PoisonRes_Mod</t>
+  </si>
+  <si>
+    <t>Armor__Amulet_Boost_STR_Mod</t>
+  </si>
+  <si>
+    <t>Armor_Unbreakable_Mod_Helmet</t>
+  </si>
+  <si>
+    <t>Armor__Helmet_Boost_PER_Mod</t>
+  </si>
+  <si>
+    <t>Armor_Gloves_DefenseValue_ArmorBoost_Normal</t>
+  </si>
+  <si>
+    <t>Armor__Gloves_Boost_Lockpicking_Mod</t>
+  </si>
+  <si>
+    <t>Armor__Body_Boost_Movement_Mod_Mid</t>
+  </si>
+  <si>
+    <t>Armor_Unbreakable_Mod_Plate</t>
+  </si>
+  <si>
+    <t>Weapon_Cripple_WeaponBoost_Axe</t>
+  </si>
+  <si>
+    <t>Weapon_Normal_Damage_Mod_2H</t>
+  </si>
+  <si>
+    <t>Armor__Ring_Boost_PoisonRes_Mod</t>
+  </si>
+  <si>
+    <t>Armor_Gloves_ReflectMelee</t>
+  </si>
+  <si>
+    <t>Armor_Gloves_DefenseValue_ArmorBoost_Normal_Mid</t>
+  </si>
+  <si>
+    <t>Armor__Garment_Boost_EarthRes_ModLarge</t>
+  </si>
+  <si>
+    <t>Armor__Garment_Boost_VitalityBoost_Mod_LargeEarly</t>
+  </si>
+  <si>
+    <t>Armor__Garment_Boost_WaterRes_Mod</t>
+  </si>
+  <si>
+    <t>Armor__Shoes_Boost_Sneaking_Mod</t>
+  </si>
+  <si>
+    <t>Armor__Shoes_Boost_VitalityBoost_Mod_Large_Late</t>
+  </si>
+  <si>
+    <t>Armor__Belt_Boost_STR_Mod</t>
+  </si>
+  <si>
+    <t>Armor__Belt_Boost_Lockpicking_Mod</t>
+  </si>
+  <si>
+    <t>Armor__Belt_Boost_Initiative_Mod_Mid</t>
+  </si>
+  <si>
+    <t>Armor__Armor_Boost_SlowedImmunity</t>
+  </si>
+  <si>
+    <t>Armor__Shoes_Boost_VitalityBoost_Mod_Large</t>
+  </si>
+  <si>
+    <t>Armor__Shoes_Boost_Movement_Mod_Medium</t>
+  </si>
+  <si>
+    <t>Armor__HelmetBoost_Initiative_Mod</t>
+  </si>
+  <si>
+    <t>Armor_Helmet_Small_ArmorDefense_Mod</t>
+  </si>
+  <si>
+    <t>Armor__Body_Boost_DEX_Mod</t>
+  </si>
+  <si>
+    <t>Armor__Body_Boost_EarthRes_ModNormal</t>
+  </si>
+  <si>
+    <t>Armor__Body_Boost_VitalityBoost_Mod_Mid</t>
+  </si>
+  <si>
+    <t>Armor__Gloves_Boost_Ranged_Mod</t>
+  </si>
+  <si>
+    <t>Armor__Gloves_Boost_Repair_Mod</t>
+  </si>
+  <si>
+    <t>Armor__Gloves_Boost_Crafting_Mod</t>
+  </si>
+  <si>
+    <t>Weapon_Large_Vitality_Mod</t>
+  </si>
+  <si>
+    <t>Weapon_Small_Damage_Mod_ModKnife</t>
+  </si>
+  <si>
+    <t>Weapon_Movement_Dagger_WeaponBoost_Late</t>
+  </si>
+  <si>
+    <t>Armor_Boost_DEX_Mod_Ring</t>
+  </si>
+  <si>
+    <t>Weapon_Large_WaterDamage_ModKnife</t>
+  </si>
+  <si>
+    <t>Weapon_Movement_Dagger_WeaponBoost_Huge_Late</t>
+  </si>
+  <si>
+    <t>Weapon_Small_FireDamage_ModKnife</t>
+  </si>
+  <si>
+    <t>Armor__Garment_Boost_AirRes_ModLarge</t>
+  </si>
+  <si>
+    <t>Armor__Garment_Boost_WaterRes_ModLarge</t>
+  </si>
+  <si>
+    <t>Armor__Ring_Boost_Movement_Mod_Medium</t>
+  </si>
+  <si>
+    <t>Armor__Helmet_Boost_VitalityBoost_Mod</t>
+  </si>
+  <si>
+    <t>Armor__Helmet_Boost_Leadership_Mod</t>
+  </si>
+  <si>
+    <t>Armor__Body_Boost_AirRes_ModNormal</t>
+  </si>
+  <si>
+    <t>Armor__Belt_Boost_BodyBuilding_Mod</t>
+  </si>
+  <si>
+    <t>Armor__Belt_Boost_Crafting_Mod</t>
+  </si>
+  <si>
+    <t>Weapon_Large_EarthDamage_ModBow</t>
+  </si>
+  <si>
+    <t>Weapon_Small_Damage_Mod_2H</t>
+  </si>
+  <si>
+    <t>Weapon_Crit_Huge_WeaponBoost</t>
+  </si>
+  <si>
+    <t>Weapon_Leadership_Mod</t>
+  </si>
+  <si>
+    <t>Weapon_Small_WaterDamage_ModBow</t>
+  </si>
+  <si>
+    <t>Armor__Gloves_Boost_Pickpocket_Mod</t>
+  </si>
+  <si>
+    <t>Weapon_Small_Vitality_Mod</t>
+  </si>
+  <si>
+    <t>Armor__Ring_Boost_PER_Mod</t>
+  </si>
+  <si>
+    <t>Armor_Small_AirResistance_ModAmulet</t>
+  </si>
+  <si>
+    <t>Armor__Ring_Boost_Movement_Mod</t>
+  </si>
+  <si>
+    <t>Weapon_Large_EarthDamage_ModKnife</t>
+  </si>
+  <si>
+    <t>Armor_Shoes_DefenseValue_Medium_ArmorBoost_Early</t>
+  </si>
+  <si>
+    <t>Armor__Shoes_Boost_Air_ModLarge</t>
+  </si>
+  <si>
+    <t>Weapon_Large_FireDamage_ModKnife</t>
+  </si>
+  <si>
+    <t>Weapon_Movement_Dagger_WeaponBoost_Large_Late</t>
+  </si>
+  <si>
+    <t>Weapon_Large_Crit_Mod_Early</t>
+  </si>
+  <si>
+    <t>Armor__Gloves_Boost_Telekinesis_Mod</t>
+  </si>
+  <si>
+    <t>Armor__Gloves_Boost_Initiative_Mod</t>
+  </si>
+  <si>
+    <t>Armor__Body_Boost_PER_Mod</t>
+  </si>
+  <si>
+    <t>Armor__Body_Boost_VitalityBoost_Mod_LargeMid</t>
+  </si>
+  <si>
+    <t>Armor__Shoes_Boost_Water_ModLarge</t>
+  </si>
+  <si>
+    <t>Armor_Belt_Boost_PoisonRes_ModLarge</t>
+  </si>
+  <si>
+    <t>Armor_Belt_Boost_VitalityBoost_Mod</t>
+  </si>
+  <si>
+    <t>Weapon_Small_EarthDamage_ModKnife</t>
+  </si>
+  <si>
+    <t>Armor_Belt_Boost_PoisonRes_Mod</t>
+  </si>
+  <si>
+    <t>Armor__Garment_Boost_FireRes_Mod</t>
+  </si>
+  <si>
+    <t>Armor__Garment_Boost_PoisonRes_Mod</t>
+  </si>
+  <si>
+    <t>Armor_Large_FireResistance_ModRing</t>
+  </si>
+  <si>
+    <t>Armor_Small_EarthResistance_ModRing</t>
+  </si>
+  <si>
+    <t>Armor__Ring_Boost_PoisonRes_Mod_Large</t>
+  </si>
+  <si>
+    <t>Armor__Shoes_Boost_Earth_ModLarge</t>
+  </si>
+  <si>
+    <t>Armor__Belt_Boost_Repair_Mod</t>
+  </si>
+  <si>
+    <t>Armor_Small_WaterResistance_ModRing</t>
+  </si>
+  <si>
+    <t>Armor__Ring_Boost_Loremaster_Mod</t>
+  </si>
+  <si>
+    <t>Armor__Amulet_Boost_Charisma_Mod</t>
+  </si>
+  <si>
+    <t>Armor__Amulet_Boost_Initiative_Mod</t>
+  </si>
+  <si>
+    <t>Armor__Body_Boost_WaterRes_ModNormal_Late</t>
+  </si>
+  <si>
+    <t>Armor__Body_Boost_EarthRes_ModNormal_Late</t>
+  </si>
+  <si>
+    <t>Weapon_Mute_Large_WeaponBoost_Wand</t>
+  </si>
+  <si>
+    <t>Weapon_Damage_Mod_Wand</t>
+  </si>
+  <si>
+    <t>Armor_Boost_Projectile_FlareStartRing</t>
+  </si>
+  <si>
+    <t>Armor_Small_AirResistance_ModRing</t>
+  </si>
+  <si>
+    <t>Armor__Shoes_Boost_Barter_Mod</t>
+  </si>
+  <si>
+    <t>Armor__Shoes_Boost_VitalityBoost_Mod</t>
+  </si>
+  <si>
+    <t>Weapon_Giant_Vitality_Mod_Mid</t>
+  </si>
+  <si>
+    <t>Weapon_Medium_Damage_Mod_Wand</t>
+  </si>
+  <si>
+    <t>Armor_Boost_Target_Fortify</t>
+  </si>
+  <si>
+    <t>Armor_Belt_Boost_VitalityBoost_Mod_LargeEarly</t>
+  </si>
+  <si>
+    <t>Armor_Gloves_Boost_VitalityBoost_Mod_LargeEarly</t>
+  </si>
+  <si>
+    <t>Armor_Shield_Air_Amulet</t>
+  </si>
+  <si>
+    <t>Armor_Path_Firefly_Garment</t>
+  </si>
+  <si>
+    <t>Weapon_Small_Speed_Mod</t>
+  </si>
+  <si>
+    <t>Ring</t>
+  </si>
+  <si>
+    <t>Weapon</t>
+  </si>
+  <si>
+    <t>Amulet</t>
+  </si>
+  <si>
+    <t>Helmet</t>
+  </si>
+  <si>
+    <t>PER</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>Mid</t>
+  </si>
+  <si>
+    <t>VitalityBoost</t>
+  </si>
+  <si>
+    <t>LargeEarly</t>
+  </si>
+  <si>
+    <t>Initiative</t>
+  </si>
+  <si>
+    <t>2H Sword</t>
+  </si>
+  <si>
+    <t>_Boost_PER_Mod</t>
+  </si>
+  <si>
+    <t>Armor__Helmet_Boost_</t>
+  </si>
+  <si>
+    <t>_Mod_</t>
+  </si>
+  <si>
+    <t>Armor__HelmetBoost_</t>
+  </si>
+  <si>
+    <t>Armor__Armor_Boost_BlindImmunity</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>",</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,6 +776,21 @@
       <color rgb="FF000000"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -430,14 +813,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -755,7 +1146,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0297D3B8-3EF5-4BD2-B114-399964914ACD}">
   <dimension ref="A1:U34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="U26" sqref="Q26:U28"/>
     </sheetView>
   </sheetViews>
@@ -784,15 +1175,15 @@
       <c r="C1" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="2"/>
-      <c r="K1" s="1" t="s">
+      <c r="H1" s="3"/>
+      <c r="I1" s="1"/>
+      <c r="K1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="1"/>
+      <c r="L1" s="3"/>
       <c r="Q1" t="s">
         <v>116</v>
       </c>
@@ -1050,14 +1441,14 @@
       <c r="C9" t="s">
         <v>65</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="H9" s="1"/>
-      <c r="K9" s="1" t="s">
+      <c r="H9" s="3"/>
+      <c r="K9" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="L9" s="1"/>
+      <c r="L9" s="3"/>
       <c r="Q9" t="s">
         <v>116</v>
       </c>
@@ -1381,14 +1772,14 @@
       <c r="C19" t="s">
         <v>66</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H19" s="1"/>
-      <c r="K19" s="1" t="s">
+      <c r="H19" s="3"/>
+      <c r="K19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="L19" s="1"/>
+      <c r="L19" s="3"/>
       <c r="Q19" t="s">
         <v>116</v>
       </c>
@@ -2106,11 +2497,1415 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="3">
+      <c r="A1" s="2">
         <v>67108864</v>
       </c>
       <c r="B1" t="s">
         <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB74B47-8327-4D53-B3EE-37D354427432}">
+  <dimension ref="A1:Q103"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="10" max="10" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="37.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" t="s">
+        <v>241</v>
+      </c>
+      <c r="J1" t="s">
+        <v>224</v>
+      </c>
+      <c r="L1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" t="s">
+        <v>241</v>
+      </c>
+      <c r="J2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L2" t="s">
+        <v>125</v>
+      </c>
+      <c r="O2" t="s">
+        <v>121</v>
+      </c>
+      <c r="P2" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" t="s">
+        <v>241</v>
+      </c>
+      <c r="J3" t="s">
+        <v>122</v>
+      </c>
+      <c r="L3" t="s">
+        <v>126</v>
+      </c>
+      <c r="P3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" t="s">
+        <v>240</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" t="s">
+        <v>241</v>
+      </c>
+      <c r="P4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" t="s">
+        <v>240</v>
+      </c>
+      <c r="B5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" t="s">
+        <v>240</v>
+      </c>
+      <c r="B6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" t="s">
+        <v>240</v>
+      </c>
+      <c r="B7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" t="s">
+        <v>240</v>
+      </c>
+      <c r="B8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" t="s">
+        <v>240</v>
+      </c>
+      <c r="B9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" t="s">
+        <v>240</v>
+      </c>
+      <c r="B10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C10" t="s">
+        <v>241</v>
+      </c>
+      <c r="J10" t="s">
+        <v>234</v>
+      </c>
+      <c r="L10" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" t="s">
+        <v>240</v>
+      </c>
+      <c r="B11" t="s">
+        <v>131</v>
+      </c>
+      <c r="C11" t="s">
+        <v>241</v>
+      </c>
+      <c r="J11" t="s">
+        <v>123</v>
+      </c>
+      <c r="L11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" t="s">
+        <v>240</v>
+      </c>
+      <c r="B12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C12" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" t="s">
+        <v>240</v>
+      </c>
+      <c r="B13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" t="s">
+        <v>240</v>
+      </c>
+      <c r="B14" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" t="s">
+        <v>240</v>
+      </c>
+      <c r="B15" t="s">
+        <v>135</v>
+      </c>
+      <c r="C15" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" t="s">
+        <v>240</v>
+      </c>
+      <c r="B16" t="s">
+        <v>136</v>
+      </c>
+      <c r="C16" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>240</v>
+      </c>
+      <c r="B17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C17" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>240</v>
+      </c>
+      <c r="B18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C18" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>240</v>
+      </c>
+      <c r="B19" t="s">
+        <v>139</v>
+      </c>
+      <c r="C19" t="s">
+        <v>241</v>
+      </c>
+      <c r="J19" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
+        <v>240</v>
+      </c>
+      <c r="B20" t="s">
+        <v>140</v>
+      </c>
+      <c r="C20" t="s">
+        <v>241</v>
+      </c>
+      <c r="J20" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>240</v>
+      </c>
+      <c r="B21" t="s">
+        <v>141</v>
+      </c>
+      <c r="C21" t="s">
+        <v>241</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>240</v>
+      </c>
+      <c r="B22" t="s">
+        <v>142</v>
+      </c>
+      <c r="C22" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" t="s">
+        <v>240</v>
+      </c>
+      <c r="B23" t="s">
+        <v>143</v>
+      </c>
+      <c r="C23" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" t="s">
+        <v>240</v>
+      </c>
+      <c r="B24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C24" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" t="s">
+        <v>240</v>
+      </c>
+      <c r="B25" t="s">
+        <v>145</v>
+      </c>
+      <c r="C25" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" t="s">
+        <v>240</v>
+      </c>
+      <c r="B26" t="s">
+        <v>146</v>
+      </c>
+      <c r="C26" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" t="s">
+        <v>240</v>
+      </c>
+      <c r="B27" t="s">
+        <v>147</v>
+      </c>
+      <c r="C27" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" t="s">
+        <v>240</v>
+      </c>
+      <c r="B28" t="s">
+        <v>148</v>
+      </c>
+      <c r="C28" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" t="s">
+        <v>240</v>
+      </c>
+      <c r="B29" t="s">
+        <v>149</v>
+      </c>
+      <c r="C29" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" t="s">
+        <v>240</v>
+      </c>
+      <c r="B30" t="s">
+        <v>150</v>
+      </c>
+      <c r="C30" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" t="s">
+        <v>240</v>
+      </c>
+      <c r="B31" t="s">
+        <v>151</v>
+      </c>
+      <c r="C31" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" t="s">
+        <v>240</v>
+      </c>
+      <c r="B32" t="s">
+        <v>152</v>
+      </c>
+      <c r="C32" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>240</v>
+      </c>
+      <c r="B33" t="s">
+        <v>153</v>
+      </c>
+      <c r="C33" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>240</v>
+      </c>
+      <c r="B34" t="s">
+        <v>154</v>
+      </c>
+      <c r="C34" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>240</v>
+      </c>
+      <c r="B35" t="s">
+        <v>155</v>
+      </c>
+      <c r="C35" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>240</v>
+      </c>
+      <c r="B36" t="s">
+        <v>156</v>
+      </c>
+      <c r="C36" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>240</v>
+      </c>
+      <c r="B37" t="s">
+        <v>157</v>
+      </c>
+      <c r="C37" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>240</v>
+      </c>
+      <c r="B38" t="s">
+        <v>158</v>
+      </c>
+      <c r="C38" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>240</v>
+      </c>
+      <c r="B39" t="s">
+        <v>159</v>
+      </c>
+      <c r="C39" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>240</v>
+      </c>
+      <c r="B40" t="s">
+        <v>160</v>
+      </c>
+      <c r="C40" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>240</v>
+      </c>
+      <c r="B41" t="s">
+        <v>161</v>
+      </c>
+      <c r="C41" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>240</v>
+      </c>
+      <c r="B42" t="s">
+        <v>162</v>
+      </c>
+      <c r="C42" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>240</v>
+      </c>
+      <c r="B43" t="s">
+        <v>163</v>
+      </c>
+      <c r="C43" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>240</v>
+      </c>
+      <c r="B44" t="s">
+        <v>164</v>
+      </c>
+      <c r="C44" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>240</v>
+      </c>
+      <c r="B45" t="s">
+        <v>165</v>
+      </c>
+      <c r="C45" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>240</v>
+      </c>
+      <c r="B46" t="s">
+        <v>166</v>
+      </c>
+      <c r="C46" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>240</v>
+      </c>
+      <c r="B47" t="s">
+        <v>167</v>
+      </c>
+      <c r="C47" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>240</v>
+      </c>
+      <c r="B48" t="s">
+        <v>168</v>
+      </c>
+      <c r="C48" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>240</v>
+      </c>
+      <c r="B49" t="s">
+        <v>169</v>
+      </c>
+      <c r="C49" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>240</v>
+      </c>
+      <c r="B50" t="s">
+        <v>170</v>
+      </c>
+      <c r="C50" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>240</v>
+      </c>
+      <c r="B51" t="s">
+        <v>171</v>
+      </c>
+      <c r="C51" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>240</v>
+      </c>
+      <c r="B52" t="s">
+        <v>172</v>
+      </c>
+      <c r="C52" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>240</v>
+      </c>
+      <c r="B53" t="s">
+        <v>173</v>
+      </c>
+      <c r="C53" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>240</v>
+      </c>
+      <c r="B54" t="s">
+        <v>174</v>
+      </c>
+      <c r="C54" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>240</v>
+      </c>
+      <c r="B55" t="s">
+        <v>175</v>
+      </c>
+      <c r="C55" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>240</v>
+      </c>
+      <c r="B56" t="s">
+        <v>176</v>
+      </c>
+      <c r="C56" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>240</v>
+      </c>
+      <c r="B57" t="s">
+        <v>177</v>
+      </c>
+      <c r="C57" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>240</v>
+      </c>
+      <c r="B58" t="s">
+        <v>178</v>
+      </c>
+      <c r="C58" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>240</v>
+      </c>
+      <c r="B59" t="s">
+        <v>179</v>
+      </c>
+      <c r="C59" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>240</v>
+      </c>
+      <c r="B60" t="s">
+        <v>180</v>
+      </c>
+      <c r="C60" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>240</v>
+      </c>
+      <c r="B61" t="s">
+        <v>181</v>
+      </c>
+      <c r="C61" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>240</v>
+      </c>
+      <c r="B62" t="s">
+        <v>182</v>
+      </c>
+      <c r="C62" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>240</v>
+      </c>
+      <c r="B63" t="s">
+        <v>183</v>
+      </c>
+      <c r="C63" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>240</v>
+      </c>
+      <c r="B64" t="s">
+        <v>184</v>
+      </c>
+      <c r="C64" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>240</v>
+      </c>
+      <c r="B65" t="s">
+        <v>185</v>
+      </c>
+      <c r="C65" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>240</v>
+      </c>
+      <c r="B66" t="s">
+        <v>186</v>
+      </c>
+      <c r="C66" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>240</v>
+      </c>
+      <c r="B67" t="s">
+        <v>187</v>
+      </c>
+      <c r="C67" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>240</v>
+      </c>
+      <c r="B68" t="s">
+        <v>188</v>
+      </c>
+      <c r="C68" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>240</v>
+      </c>
+      <c r="B69" t="s">
+        <v>189</v>
+      </c>
+      <c r="C69" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>240</v>
+      </c>
+      <c r="B70" t="s">
+        <v>190</v>
+      </c>
+      <c r="C70" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>240</v>
+      </c>
+      <c r="B71" t="s">
+        <v>191</v>
+      </c>
+      <c r="C71" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>240</v>
+      </c>
+      <c r="B72" t="s">
+        <v>192</v>
+      </c>
+      <c r="C72" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>240</v>
+      </c>
+      <c r="B73" t="s">
+        <v>193</v>
+      </c>
+      <c r="C73" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>240</v>
+      </c>
+      <c r="B74" t="s">
+        <v>194</v>
+      </c>
+      <c r="C74" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>240</v>
+      </c>
+      <c r="B75" t="s">
+        <v>195</v>
+      </c>
+      <c r="C75" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>240</v>
+      </c>
+      <c r="B76" t="s">
+        <v>196</v>
+      </c>
+      <c r="C76" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>240</v>
+      </c>
+      <c r="B77" t="s">
+        <v>197</v>
+      </c>
+      <c r="C77" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>240</v>
+      </c>
+      <c r="B78" t="s">
+        <v>198</v>
+      </c>
+      <c r="C78" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>240</v>
+      </c>
+      <c r="B79" t="s">
+        <v>199</v>
+      </c>
+      <c r="C79" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>240</v>
+      </c>
+      <c r="B80" t="s">
+        <v>200</v>
+      </c>
+      <c r="C80" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>240</v>
+      </c>
+      <c r="B81" t="s">
+        <v>201</v>
+      </c>
+      <c r="C81" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>240</v>
+      </c>
+      <c r="B82" t="s">
+        <v>202</v>
+      </c>
+      <c r="C82" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>240</v>
+      </c>
+      <c r="B83" t="s">
+        <v>203</v>
+      </c>
+      <c r="C83" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>240</v>
+      </c>
+      <c r="B84" t="s">
+        <v>204</v>
+      </c>
+      <c r="C84" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>240</v>
+      </c>
+      <c r="B85" t="s">
+        <v>205</v>
+      </c>
+      <c r="C85" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>240</v>
+      </c>
+      <c r="B86" t="s">
+        <v>206</v>
+      </c>
+      <c r="C86" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>240</v>
+      </c>
+      <c r="B87" t="s">
+        <v>207</v>
+      </c>
+      <c r="C87" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>240</v>
+      </c>
+      <c r="B88" t="s">
+        <v>208</v>
+      </c>
+      <c r="C88" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
+        <v>240</v>
+      </c>
+      <c r="B89" t="s">
+        <v>209</v>
+      </c>
+      <c r="C89" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>240</v>
+      </c>
+      <c r="B90" t="s">
+        <v>210</v>
+      </c>
+      <c r="C90" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>240</v>
+      </c>
+      <c r="B91" t="s">
+        <v>211</v>
+      </c>
+      <c r="C91" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
+        <v>240</v>
+      </c>
+      <c r="B92" t="s">
+        <v>212</v>
+      </c>
+      <c r="C92" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
+        <v>240</v>
+      </c>
+      <c r="B93" t="s">
+        <v>213</v>
+      </c>
+      <c r="C93" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
+        <v>240</v>
+      </c>
+      <c r="B94" t="s">
+        <v>214</v>
+      </c>
+      <c r="C94" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" t="s">
+        <v>240</v>
+      </c>
+      <c r="B95" t="s">
+        <v>215</v>
+      </c>
+      <c r="C95" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" t="s">
+        <v>240</v>
+      </c>
+      <c r="B96" t="s">
+        <v>216</v>
+      </c>
+      <c r="C96" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
+        <v>240</v>
+      </c>
+      <c r="B97" t="s">
+        <v>217</v>
+      </c>
+      <c r="C97" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" t="s">
+        <v>240</v>
+      </c>
+      <c r="B98" t="s">
+        <v>218</v>
+      </c>
+      <c r="C98" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" t="s">
+        <v>240</v>
+      </c>
+      <c r="B99" t="s">
+        <v>219</v>
+      </c>
+      <c r="C99" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" t="s">
+        <v>240</v>
+      </c>
+      <c r="B100" t="s">
+        <v>220</v>
+      </c>
+      <c r="C100" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" t="s">
+        <v>240</v>
+      </c>
+      <c r="B101" t="s">
+        <v>221</v>
+      </c>
+      <c r="C101" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" t="s">
+        <v>240</v>
+      </c>
+      <c r="B102" t="s">
+        <v>222</v>
+      </c>
+      <c r="C102" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" t="s">
+        <v>240</v>
+      </c>
+      <c r="B103" t="s">
+        <v>223</v>
+      </c>
+      <c r="C103" t="s">
+        <v>241</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DCC817B-14F6-472C-AAF0-0D510F97842B}">
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B4" t="s">
+        <v>228</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Added Traits tab - Added an apply button so user can apply any changes to the currently editing character before selecting another one. - Added support for directly loading savegame from dumped json, making debug faster
</commit_message>
<xml_diff>
--- a/xml scheme.xlsx
+++ b/xml scheme.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Visual Studio 2017\Projects\D-OS SE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6799634D-6A39-4392-A32B-9D557B248801}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD0A999-5349-4CDE-A6B1-3BEDDA48B1EA}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23190" windowHeight="10815" activeTab="4" xr2:uid="{74786857-5191-4C0D-86D0-001FA1C9B969}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23190" windowHeight="10815" activeTab="2" xr2:uid="{74786857-5191-4C0D-86D0-001FA1C9B969}"/>
   </bookViews>
   <sheets>
     <sheet name="Abilities" sheetId="1" r:id="rId1"/>
     <sheet name="Attributes" sheetId="4" r:id="rId2"/>
     <sheet name="Traits" sheetId="2" r:id="rId3"/>
-    <sheet name="Talent" sheetId="3" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="7" r:id="rId4"/>
+    <sheet name="Talent" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="281">
   <si>
     <t>bow</t>
   </si>
@@ -756,6 +757,123 @@
   </si>
   <si>
     <t>",</t>
+  </si>
+  <si>
+    <t>&lt;TextBlock</t>
+  </si>
+  <si>
+    <t>Grid.Row</t>
+  </si>
+  <si>
+    <t>Grid.Column</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>HorizontalAlignment</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>ToolTip</t>
+  </si>
+  <si>
+    <t>Blunt?</t>
+  </si>
+  <si>
+    <t>Immune to Charmed/&gt;</t>
+  </si>
+  <si>
+    <t>+2 Reputation/&gt;</t>
+  </si>
+  <si>
+    <t>+1 Willpower/&gt;</t>
+  </si>
+  <si>
+    <t>+1 Crafting/&gt;</t>
+  </si>
+  <si>
+    <t>Immune to Fear/&gt;</t>
+  </si>
+  <si>
+    <t>+1 Leadership/&gt;</t>
+  </si>
+  <si>
+    <t>Bold?</t>
+  </si>
+  <si>
+    <t>+1 Initiative/&gt;</t>
+  </si>
+  <si>
+    <t>+3% Critical Chance/&gt;</t>
+  </si>
+  <si>
+    <t>+20% chance to hit on attacks of opportunity/&gt;</t>
+  </si>
+  <si>
+    <t>Considerate?</t>
+  </si>
+  <si>
+    <t>+1 Charisma/&gt;</t>
+  </si>
+  <si>
+    <t>+1 Bartering/&gt;</t>
+  </si>
+  <si>
+    <t>+1 Willpower when an ally with Leadership is in sight (+2 Willpower if ally has Leadership 5 or higher)/&gt;</t>
+  </si>
+  <si>
+    <t>+1 Lucky Charm/&gt;</t>
+  </si>
+  <si>
+    <t>+1 Loremaster/&gt;</t>
+  </si>
+  <si>
+    <t>+1 Pickpocketing/&gt;</t>
+  </si>
+  <si>
+    <t>Cautious?</t>
+  </si>
+  <si>
+    <t>+1 Sneaking/&gt;</t>
+  </si>
+  <si>
+    <t>+20% chance to hit when backstabbing/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;TextBox</t>
+  </si>
+  <si>
+    <t>x:Name</t>
+  </si>
+  <si>
+    <t>FogivingTextBox</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>20/&gt;</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>TraitCouple(</t>
+  </si>
+  <si>
+    <t>Trait("Forgiving",</t>
+  </si>
+  <si>
+    <t>1,</t>
+  </si>
+  <si>
+    <t>Immune to Cursed),</t>
+  </si>
+  <si>
+    <t>Immune to Cursed));</t>
   </si>
 </sst>
 </file>
@@ -820,15 +938,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1175,15 +1293,15 @@
       <c r="C1" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="3"/>
+      <c r="H1" s="7"/>
       <c r="I1" s="1"/>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="3"/>
+      <c r="L1" s="7"/>
       <c r="Q1" t="s">
         <v>116</v>
       </c>
@@ -1441,14 +1559,14 @@
       <c r="C9" t="s">
         <v>65</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H9" s="3"/>
-      <c r="K9" s="3" t="s">
+      <c r="H9" s="7"/>
+      <c r="K9" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="L9" s="3"/>
+      <c r="L9" s="7"/>
       <c r="Q9" t="s">
         <v>116</v>
       </c>
@@ -1772,14 +1890,14 @@
       <c r="C19" t="s">
         <v>66</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="H19" s="3"/>
-      <c r="K19" s="3" t="s">
+      <c r="H19" s="7"/>
+      <c r="K19" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="L19" s="3"/>
+      <c r="L19" s="7"/>
       <c r="Q19" t="s">
         <v>116</v>
       </c>
@@ -2270,10 +2388,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD8E76CB-E14A-4496-A7AB-230CDEAAA37F}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2458,7 +2576,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2466,7 +2584,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2475,6 +2593,851 @@
       </c>
       <c r="C18" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="B24" t="s">
+        <v>240</v>
+      </c>
+      <c r="C24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="B25" t="s">
+        <v>240</v>
+      </c>
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="B26" t="s">
+        <v>240</v>
+      </c>
+      <c r="C26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="B27" t="s">
+        <v>240</v>
+      </c>
+      <c r="C27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="B28" t="s">
+        <v>240</v>
+      </c>
+      <c r="C28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="B29" t="s">
+        <v>240</v>
+      </c>
+      <c r="C29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="B30" t="s">
+        <v>240</v>
+      </c>
+      <c r="C30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="B31" t="s">
+        <v>240</v>
+      </c>
+      <c r="C31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="B32" t="s">
+        <v>240</v>
+      </c>
+      <c r="C32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" t="s">
+        <v>240</v>
+      </c>
+      <c r="C33" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="B34" t="s">
+        <v>240</v>
+      </c>
+      <c r="C34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="B35" t="s">
+        <v>240</v>
+      </c>
+      <c r="C35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4">
+      <c r="B36" t="s">
+        <v>240</v>
+      </c>
+      <c r="C36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4">
+      <c r="B37" t="s">
+        <v>240</v>
+      </c>
+      <c r="C37" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4">
+      <c r="B38" t="s">
+        <v>240</v>
+      </c>
+      <c r="C38" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4">
+      <c r="B39" t="s">
+        <v>240</v>
+      </c>
+      <c r="C39" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4">
+      <c r="B40" t="s">
+        <v>240</v>
+      </c>
+      <c r="C40" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4">
+      <c r="B41" t="s">
+        <v>240</v>
+      </c>
+      <c r="C41" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4">
+      <c r="C43" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4">
+      <c r="C44" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6E1002A-AC0B-470A-AA6C-B936890881CF}">
+  <dimension ref="B2:N30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="2:12">
+      <c r="B2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C2" t="s">
+        <v>243</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>244</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>245</v>
+      </c>
+      <c r="H2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I2" t="s">
+        <v>246</v>
+      </c>
+      <c r="J2" t="s">
+        <v>247</v>
+      </c>
+      <c r="K2" t="s">
+        <v>248</v>
+      </c>
+      <c r="L2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12">
+      <c r="B3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C3" t="s">
+        <v>243</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>245</v>
+      </c>
+      <c r="H3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" t="s">
+        <v>246</v>
+      </c>
+      <c r="J3" t="s">
+        <v>247</v>
+      </c>
+      <c r="K3" t="s">
+        <v>248</v>
+      </c>
+      <c r="L3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12">
+      <c r="B4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C4" t="s">
+        <v>243</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>244</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>245</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" t="s">
+        <v>246</v>
+      </c>
+      <c r="J4" t="s">
+        <v>247</v>
+      </c>
+      <c r="K4" t="s">
+        <v>248</v>
+      </c>
+      <c r="L4" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12">
+      <c r="B5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C5" t="s">
+        <v>243</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>244</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>245</v>
+      </c>
+      <c r="H5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" t="s">
+        <v>246</v>
+      </c>
+      <c r="J5" t="s">
+        <v>247</v>
+      </c>
+      <c r="K5" t="s">
+        <v>248</v>
+      </c>
+      <c r="L5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12">
+      <c r="B6" t="s">
+        <v>242</v>
+      </c>
+      <c r="C6" t="s">
+        <v>243</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>244</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>245</v>
+      </c>
+      <c r="H6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" t="s">
+        <v>246</v>
+      </c>
+      <c r="J6" t="s">
+        <v>247</v>
+      </c>
+      <c r="K6" t="s">
+        <v>248</v>
+      </c>
+      <c r="L6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
+      <c r="B7" t="s">
+        <v>242</v>
+      </c>
+      <c r="C7" t="s">
+        <v>243</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>244</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>245</v>
+      </c>
+      <c r="H7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" t="s">
+        <v>246</v>
+      </c>
+      <c r="J7" t="s">
+        <v>247</v>
+      </c>
+      <c r="K7" t="s">
+        <v>248</v>
+      </c>
+      <c r="L7" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12">
+      <c r="B8" t="s">
+        <v>242</v>
+      </c>
+      <c r="C8" t="s">
+        <v>243</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>244</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>245</v>
+      </c>
+      <c r="H8" t="s">
+        <v>256</v>
+      </c>
+      <c r="I8" t="s">
+        <v>246</v>
+      </c>
+      <c r="J8" t="s">
+        <v>247</v>
+      </c>
+      <c r="K8" t="s">
+        <v>248</v>
+      </c>
+      <c r="L8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12">
+      <c r="B9" t="s">
+        <v>242</v>
+      </c>
+      <c r="C9" t="s">
+        <v>243</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>244</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>245</v>
+      </c>
+      <c r="H9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" t="s">
+        <v>246</v>
+      </c>
+      <c r="J9" t="s">
+        <v>247</v>
+      </c>
+      <c r="K9" t="s">
+        <v>248</v>
+      </c>
+      <c r="L9" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12">
+      <c r="B10" t="s">
+        <v>242</v>
+      </c>
+      <c r="C10" t="s">
+        <v>243</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>244</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10" t="s">
+        <v>245</v>
+      </c>
+      <c r="H10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" t="s">
+        <v>248</v>
+      </c>
+      <c r="J10" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12">
+      <c r="B11" t="s">
+        <v>242</v>
+      </c>
+      <c r="C11" t="s">
+        <v>243</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>244</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11" t="s">
+        <v>245</v>
+      </c>
+      <c r="H11" t="s">
+        <v>260</v>
+      </c>
+      <c r="I11" t="s">
+        <v>248</v>
+      </c>
+      <c r="J11" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12">
+      <c r="B12" t="s">
+        <v>242</v>
+      </c>
+      <c r="C12" t="s">
+        <v>243</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>244</v>
+      </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="G12" t="s">
+        <v>245</v>
+      </c>
+      <c r="H12" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" t="s">
+        <v>248</v>
+      </c>
+      <c r="J12" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12">
+      <c r="B13" t="s">
+        <v>242</v>
+      </c>
+      <c r="C13" t="s">
+        <v>243</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>244</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="G13" t="s">
+        <v>245</v>
+      </c>
+      <c r="H13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" t="s">
+        <v>248</v>
+      </c>
+      <c r="J13" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12">
+      <c r="B14" t="s">
+        <v>242</v>
+      </c>
+      <c r="C14" t="s">
+        <v>243</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>244</v>
+      </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
+      <c r="G14" t="s">
+        <v>245</v>
+      </c>
+      <c r="H14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" t="s">
+        <v>248</v>
+      </c>
+      <c r="J14" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12">
+      <c r="B15" t="s">
+        <v>242</v>
+      </c>
+      <c r="C15" t="s">
+        <v>243</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>244</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
+      <c r="G15" t="s">
+        <v>245</v>
+      </c>
+      <c r="H15" t="s">
+        <v>45</v>
+      </c>
+      <c r="I15" t="s">
+        <v>248</v>
+      </c>
+      <c r="J15" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12">
+      <c r="B16" t="s">
+        <v>242</v>
+      </c>
+      <c r="C16" t="s">
+        <v>243</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>244</v>
+      </c>
+      <c r="F16">
+        <v>4</v>
+      </c>
+      <c r="G16" t="s">
+        <v>245</v>
+      </c>
+      <c r="H16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" t="s">
+        <v>248</v>
+      </c>
+      <c r="J16" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14">
+      <c r="B17" t="s">
+        <v>242</v>
+      </c>
+      <c r="C17" t="s">
+        <v>243</v>
+      </c>
+      <c r="D17">
+        <v>7</v>
+      </c>
+      <c r="E17" t="s">
+        <v>244</v>
+      </c>
+      <c r="F17">
+        <v>4</v>
+      </c>
+      <c r="G17" t="s">
+        <v>245</v>
+      </c>
+      <c r="H17" t="s">
+        <v>267</v>
+      </c>
+      <c r="I17" t="s">
+        <v>248</v>
+      </c>
+      <c r="J17" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14">
+      <c r="B18" t="s">
+        <v>242</v>
+      </c>
+      <c r="C18" t="s">
+        <v>243</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
+        <v>244</v>
+      </c>
+      <c r="F18">
+        <v>4</v>
+      </c>
+      <c r="G18" t="s">
+        <v>245</v>
+      </c>
+      <c r="H18" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" t="s">
+        <v>248</v>
+      </c>
+      <c r="J18" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14">
+      <c r="B19" t="s">
+        <v>270</v>
+      </c>
+      <c r="C19" t="s">
+        <v>271</v>
+      </c>
+      <c r="D19" t="s">
+        <v>272</v>
+      </c>
+      <c r="E19" t="s">
+        <v>243</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
+        <v>244</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19" t="s">
+        <v>245</v>
+      </c>
+      <c r="K19" t="s">
+        <v>246</v>
+      </c>
+      <c r="L19" t="s">
+        <v>247</v>
+      </c>
+      <c r="M19" t="s">
+        <v>273</v>
+      </c>
+      <c r="N19" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14">
+      <c r="F23" t="s">
+        <v>275</v>
+      </c>
+      <c r="G23" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14">
+      <c r="G24" t="s">
+        <v>275</v>
+      </c>
+      <c r="H24" t="s">
+        <v>277</v>
+      </c>
+      <c r="I24" t="s">
+        <v>278</v>
+      </c>
+      <c r="J24" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14">
+      <c r="G25" t="s">
+        <v>275</v>
+      </c>
+      <c r="H25" t="s">
+        <v>277</v>
+      </c>
+      <c r="I25" t="s">
+        <v>278</v>
+      </c>
+      <c r="J25" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14">
+      <c r="D30" t="str">
+        <f>"StackPanel.Children.Add(new TraitCouple(new Trait("</f>
+        <v>StackPanel.Children.Add(new TraitCouple(new Trait(</v>
       </c>
     </row>
   </sheetData>
@@ -2482,7 +3445,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA4938FB-5B1A-42EF-BC41-6D1AA7DE6B88}">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -2509,11 +3472,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB74B47-8327-4D53-B3EE-37D354427432}">
   <dimension ref="A1:Q103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
@@ -2804,7 +3767,7 @@
       <c r="C21" t="s">
         <v>241</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="J21" s="3" t="s">
         <v>128</v>
       </c>
     </row>
@@ -3716,7 +4679,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DCC817B-14F6-472C-AAF0-0D510F97842B}">
   <dimension ref="A1:F20"/>
   <sheetViews>
@@ -3741,13 +4704,13 @@
       <c r="A2" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>232</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -3761,7 +4724,7 @@
       <c r="B3" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>237</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -3775,7 +4738,7 @@
       <c r="B4" t="s">
         <v>228</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>237</v>
       </c>
     </row>
@@ -3783,7 +4746,7 @@
       <c r="A5" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>237</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -3794,7 +4757,7 @@
       <c r="A6" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>237</v>
       </c>
     </row>
@@ -3802,7 +4765,7 @@
       <c r="A7" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>237</v>
       </c>
     </row>
@@ -3810,7 +4773,7 @@
       <c r="A8" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>237</v>
       </c>
     </row>
@@ -3818,7 +4781,7 @@
       <c r="A9" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>237</v>
       </c>
     </row>
@@ -3826,7 +4789,7 @@
       <c r="A10" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>237</v>
       </c>
     </row>
@@ -3834,7 +4797,7 @@
       <c r="A11" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>237</v>
       </c>
     </row>
@@ -3842,7 +4805,7 @@
       <c r="A12" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>237</v>
       </c>
     </row>
@@ -3850,7 +4813,7 @@
       <c r="A13" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>237</v>
       </c>
     </row>
@@ -3858,7 +4821,7 @@
       <c r="A14" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>237</v>
       </c>
     </row>
@@ -3866,7 +4829,7 @@
       <c r="A15" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>237</v>
       </c>
     </row>
@@ -3874,7 +4837,7 @@
       <c r="A16" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>237</v>
       </c>
     </row>
@@ -3882,7 +4845,7 @@
       <c r="A17" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>237</v>
       </c>
     </row>
@@ -3890,7 +4853,7 @@
       <c r="A18" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>237</v>
       </c>
     </row>
@@ -3898,13 +4861,13 @@
       <c r="A20" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="5" t="s">
         <v>230</v>
       </c>
     </row>

</xml_diff>